<commit_message>
tier issue in asset resolved
</commit_message>
<xml_diff>
--- a/public/assets-new/Sample_Asset_English.xlsx
+++ b/public/assets-new/Sample_Asset_English.xlsx
@@ -80,13 +80,7 @@
     <t>Website</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cloud </t>
-  </si>
-  <si>
-    <t>Not sure</t>
   </si>
   <si>
     <t>Afghanistan</t>
@@ -854,9 +848,6 @@
     <t>Data retention</t>
   </si>
   <si>
-    <t>On-premise</t>
-  </si>
-  <si>
     <r>
       <t>Asset name</t>
     </r>
@@ -954,6 +945,15 @@
   </si>
   <si>
     <t>Crown Jewels</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>On-Premise</t>
+  </si>
+  <si>
+    <t>Not Sure</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1371,7 @@
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,19 +1395,19 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>0</v>
@@ -1416,40 +1416,40 @@
         <v>1</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="N1" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>275</v>
-      </c>
       <c r="P1" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="Q1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>262</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>264</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>5</v>
@@ -3804,7 +3804,7 @@
   <dimension ref="A1:J203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3822,26 +3822,26 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -3855,22 +3855,22 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -3884,28 +3884,28 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3913,51 +3913,51 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>278</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F4" t="s">
         <v>206</v>
       </c>
-      <c r="F4" t="s">
-        <v>208</v>
-      </c>
       <c r="G4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3965,704 +3965,704 @@
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D27" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D28" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D29" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D30" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D31" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D37" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D38" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D39" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D40" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D41" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D42" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D43" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D45" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D47" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D53" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D54" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D55" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D60" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D61" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D62" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D63" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D64" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D65" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D67" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D68" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D69" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D70" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D71" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D72" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D73" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D74" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D75" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D77" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D78" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D79" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D80" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D81" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D83" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D84" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D85" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D86" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D87" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D88" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D89" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D90" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D91" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D92" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D93" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D94" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D95" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D96" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D97" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D98" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D99" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="100" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D100" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D101" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D102" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="103" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D103" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="104" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D104" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="105" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D105" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="106" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D106" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="107" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D107" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D108" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D109" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D110" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="111" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D111" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D112" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D113" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="114" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D114" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D115" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="116" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D116" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="117" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D117" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="118" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D118" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="119" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D119" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="120" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D120" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="121" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D121" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="122" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D122" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="123" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D123" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="124" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D124" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D125" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D126" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D127" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D128" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D129" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D130" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D131" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D132" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D133" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="134" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D134" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="135" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4672,337 +4672,337 @@
     </row>
     <row r="136" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D136" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="137" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D137" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="138" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D138" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="139" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D139" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="140" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D140" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="141" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D141" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="142" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D142" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="143" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D143" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="144" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D144" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="145" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D145" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="146" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D146" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="147" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D147" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="148" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D148" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="149" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D149" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="150" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D150" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="151" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D151" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="152" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D152" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D153" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="154" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D154" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="155" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D155" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="156" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D156" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="157" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D157" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="158" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D158" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="159" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D159" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="160" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D160" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="161" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D161" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="162" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D162" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D163" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="164" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D164" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="165" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D165" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="166" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D166" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="167" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D167" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="168" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D168" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="169" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D169" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="170" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D170" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="171" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D171" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="172" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D172" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="173" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D173" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="174" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D174" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="175" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D175" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="176" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D176" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="177" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D177" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="178" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D178" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="179" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D179" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="180" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D180" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="181" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D181" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="182" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D182" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="183" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D183" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="184" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D184" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="185" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D185" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="186" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D186" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="187" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D187" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="188" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D188" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="189" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D189" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="190" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D190" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="191" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D191" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="192" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D192" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="193" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D193" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="194" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D194" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="195" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D195" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="196" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D196" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="197" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D197" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="198" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D198" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="199" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D199" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="200" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D200" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="201" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D201" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="202" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D202" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="203" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -5023,17 +5023,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7fe41b35-81d4-4e31-bf5f-318b49e8a5d3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="de64d92b-4328-4b32-9550-e2f09f3419ad" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009303596CFA10E74C8743183CDC9C0378" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="62cedd2d167250fea98604144b5f3c4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7fe41b35-81d4-4e31-bf5f-318b49e8a5d3" xmlns:ns3="de64d92b-4328-4b32-9550-e2f09f3419ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="542df12b81495dad77b8b320a2a41c9c" ns2:_="" ns3:_="">
     <xsd:import namespace="7fe41b35-81d4-4e31-bf5f-318b49e8a5d3"/>
@@ -5262,6 +5251,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7fe41b35-81d4-4e31-bf5f-318b49e8a5d3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="de64d92b-4328-4b32-9550-e2f09f3419ad" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D657BA3A-32B5-4F59-8EF6-809486126D3A}">
   <ds:schemaRefs>
@@ -5271,17 +5271,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B4A77-B751-47D6-B659-274364956C6B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7fe41b35-81d4-4e31-bf5f-318b49e8a5d3"/>
-    <ds:schemaRef ds:uri="de64d92b-4328-4b32-9550-e2f09f3419ad"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0F8171-B25C-40A9-8F4D-0F179335A5C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5298,4 +5287,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B4A77-B751-47D6-B659-274364956C6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="de64d92b-4328-4b32-9550-e2f09f3419ad"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7fe41b35-81d4-4e31-bf5f-318b49e8a5d3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>